<commit_message>
Added more title cards and updated the rhythm game test fileA
</commit_message>
<xml_diff>
--- a/static/rhythm_games/TestA.xlsx
+++ b/static/rhythm_games/TestA.xlsx
@@ -82,7 +82,7 @@
     <t>Donut Remix</t>
   </si>
   <si>
-    <t>donut_remix.png</t>
+    <t>donut_remix_megamix.png</t>
   </si>
   <si>
     <t>Rat Race</t>
@@ -142,7 +142,7 @@
     <t>Fever</t>
   </si>
   <si>
-    <t>fork_lifter_2p.png</t>
+    <t>fork_lifter_2p_fever.png</t>
   </si>
   <si>
     <t>Pirate Crew</t>
@@ -151,7 +151,7 @@
     <t>2 Player Endless</t>
   </si>
   <si>
-    <t>pirate_crew.png</t>
+    <t>pirate_crew_fever.png</t>
   </si>
   <si>
     <t>Rhythm Fighter</t>
@@ -160,7 +160,7 @@
     <t>2 Player Vs</t>
   </si>
   <si>
-    <t>rhythm_fighter.png</t>
+    <t>rhythm_fighter_fever.png</t>
   </si>
 </sst>
 </file>
@@ -518,6 +518,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="7" max="7" width="24.25"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -541,11 +544,10 @@
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -571,8 +573,7 @@
       <c r="G2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>13</v>
       </c>
     </row>
@@ -598,8 +599,7 @@
       <c r="G3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -625,11 +625,10 @@
       <c r="G5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="9" t="s">
+      <c r="H5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="9" t="s">
         <v>9</v>
       </c>
     </row>
@@ -655,8 +654,7 @@
       <c r="G6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -682,20 +680,19 @@
       <c r="G7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="3"/>
+      <c r="H7" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="I7" s="2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M7" s="2" t="s">
         <v>27</v>
       </c>
     </row>
@@ -721,11 +718,10 @@
       <c r="G9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J9" s="9"/>
+      <c r="H9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="9"/>
     </row>
     <row r="10">
       <c r="A10" s="11" t="s">
@@ -749,14 +745,13 @@
       <c r="G10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3" t="s">
-        <v>12</v>
+      <c r="H10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>9</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K10" s="9" t="s">
         <v>17</v>
       </c>
     </row>
@@ -782,11 +777,10 @@
       <c r="G11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="3"/>
-      <c r="I11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J11" s="9" t="s">
+      <c r="H11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="9" t="s">
         <v>20</v>
       </c>
     </row>
@@ -812,11 +806,10 @@
       <c r="G12" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J12" s="9" t="s">
+      <c r="H12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="9" t="s">
         <v>20</v>
       </c>
     </row>
@@ -842,11 +835,10 @@
       <c r="G14" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="H14" s="9"/>
+      <c r="H14" s="9" t="s">
+        <v>12</v>
+      </c>
       <c r="I14" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="J14" s="9" t="s">
         <v>28</v>
       </c>
     </row>
@@ -872,8 +864,7 @@
       <c r="G16" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9" t="s">
+      <c r="H16" s="9" t="s">
         <v>13</v>
       </c>
     </row>
@@ -899,8 +890,7 @@
       <c r="G18" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9" t="s">
+      <c r="H18" s="9" t="s">
         <v>13</v>
       </c>
     </row>
@@ -926,8 +916,7 @@
       <c r="G20" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9" t="s">
+      <c r="H20" s="9" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added base megamix testfile and the remaining base title cards
</commit_message>
<xml_diff>
--- a/static/rhythm_games/TestA.xlsx
+++ b/static/rhythm_games/TestA.xlsx
@@ -88,10 +88,10 @@
     <t>Rat Race</t>
   </si>
   <si>
-    <t>Working Dough</t>
-  </si>
-  <si>
-    <t>Fan Club</t>
+    <t>Working Dough 1</t>
+  </si>
+  <si>
+    <t>Fan Club 1</t>
   </si>
   <si>
     <t>Animal Acrobat</t>
@@ -686,10 +686,10 @@
       <c r="I7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L7" s="2" t="s">

</xml_diff>